<commit_message>
Data addition & optimization
</commit_message>
<xml_diff>
--- a/assets/dataset/data_1.xlsx
+++ b/assets/dataset/data_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarufN\Documents\Study\UTY\materi&amp;tugas-s1_informatika\semester_6\fuzzy_logic-b\task\elearning\meet_9-group_task_fcm_clustering\added_file\system\assets\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarufN\Documents\Study\UTY\materi&amp;tugas-s1_informatika\semester_6\fuzzy_logic-b\task\elearning\meet_9-fcm_clustering\group_task\added_file\system\assets\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A3F0FC-61D3-42A4-9CE2-82EC90DBD20E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F37FADA-7A39-4D6F-8678-BBCA5E5512C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="x" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="226">
   <si>
     <t>0,198</t>
   </si>
@@ -339,21 +339,6 @@
     <t>0,150</t>
   </si>
   <si>
-    <t>0.284</t>
-  </si>
-  <si>
-    <t>0.230</t>
-  </si>
-  <si>
-    <t>0.222</t>
-  </si>
-  <si>
-    <t>0.044</t>
-  </si>
-  <si>
-    <t>0.221</t>
-  </si>
-  <si>
     <t>ORIGIN</t>
   </si>
   <si>
@@ -718,6 +703,9 @@
   </si>
   <si>
     <t>0,170</t>
+  </si>
+  <si>
+    <t>0,044</t>
   </si>
 </sst>
 </file>
@@ -930,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -996,6 +984,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1337,7 +1328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667AD196-323C-4D3D-B628-B96AB55DF13A}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -1361,28 +1352,28 @@
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="9"/>
       <c r="H1" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="M1" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="9"/>
       <c r="R1" s="20" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1390,16 +1381,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H2" s="17" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(C2,".",""), ",", "")</f>
@@ -1443,16 +1434,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H3" s="10" t="str">
         <f t="shared" ref="H3:K31" si="2">SUBSTITUTE(SUBSTITUTE(C3,".",""), ",", "")</f>
@@ -1496,16 +1487,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H4" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1549,16 +1540,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H5" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1602,16 +1593,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H6" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1655,16 +1646,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H7" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1708,13 +1699,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F8" s="13">
         <v>5000000</v>
@@ -1761,13 +1752,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F9" s="13">
         <v>8000000</v>
@@ -1814,16 +1805,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H10" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1867,16 +1858,16 @@
         <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H11" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1920,16 +1911,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="H12" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1973,16 +1964,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H13" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2026,16 +2017,16 @@
         <v>13</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H14" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2079,16 +2070,16 @@
         <v>14</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H15" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2132,16 +2123,16 @@
         <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H16" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2185,16 +2176,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H17" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2238,16 +2229,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H18" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2291,16 +2282,16 @@
         <v>18</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H19" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2344,16 +2335,16 @@
         <v>19</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H20" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2397,16 +2388,16 @@
         <v>20</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H21" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2450,16 +2441,16 @@
         <v>21</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H22" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2503,16 +2494,16 @@
         <v>22</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H23" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2556,16 +2547,16 @@
         <v>23</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H24" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2609,16 +2600,16 @@
         <v>24</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H25" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2662,16 +2653,16 @@
         <v>25</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H26" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2715,16 +2706,16 @@
         <v>26</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H27" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2768,16 +2759,16 @@
         <v>27</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H28" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2821,13 +2812,13 @@
         <v>28</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F29" s="13">
         <v>21500000</v>
@@ -2874,13 +2865,13 @@
         <v>29</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F30" s="13">
         <v>2000000</v>
@@ -2927,16 +2918,16 @@
         <v>30</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H31" s="14" t="str">
         <f t="shared" si="2"/>
@@ -2984,32 +2975,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O31" sqref="O2:O31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H31" sqref="H2:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
       <c r="G1" s="27"/>
       <c r="I1" s="25" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
       <c r="L1" s="26"/>
       <c r="M1" s="27"/>
       <c r="O1" s="23" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -3080,15 +3071,15 @@
         <v>0.153</v>
       </c>
       <c r="J3" s="32" t="str">
-        <f t="shared" ref="J3:J30" si="2">SUBSTITUTE(D3, ",", ".")</f>
+        <f t="shared" ref="J3:J27" si="2">SUBSTITUTE(D3, ",", ".")</f>
         <v>0.188</v>
       </c>
       <c r="K3" s="32" t="str">
-        <f t="shared" ref="K3:K30" si="3">SUBSTITUTE(E3, ",", ".")</f>
+        <f t="shared" ref="K3:K27" si="3">SUBSTITUTE(E3, ",", ".")</f>
         <v>0.258</v>
       </c>
       <c r="L3" s="32" t="str">
-        <f t="shared" ref="L3:L31" si="4">SUBSTITUTE(F3, ",", ".")</f>
+        <f t="shared" ref="L3:L27" si="4">SUBSTITUTE(F3, ",", ".")</f>
         <v>0.201</v>
       </c>
       <c r="M3" s="33" t="str">
@@ -4116,20 +4107,20 @@
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="C27" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>107</v>
+      <c r="C27" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="G27" s="49" t="s">
+        <v>67</v>
       </c>
       <c r="I27" s="31" t="str">
         <f t="shared" si="1"/>
@@ -4208,10 +4199,10 @@
         <v>0.187</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F29" s="39">
         <v>0.27600000000000002</v>
@@ -4255,13 +4246,13 @@
         <v>0.22800000000000001</v>
       </c>
       <c r="E30" s="40" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F30" s="39">
         <v>0.30199999999999999</v>
       </c>
       <c r="G30" s="42" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I30" s="31" t="str">
         <f t="shared" si="7"/>

</xml_diff>